<commit_message>
figured out neural network
</commit_message>
<xml_diff>
--- a/evaluation/embeddings_scores.xlsx
+++ b/evaluation/embeddings_scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acqua\Code\contextual_embeddings\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037D9B67-C7A4-4EA3-B7A6-B39481C5E6BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A746AA-DB45-423B-937B-CB7A60D61D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{C064456A-E08A-474B-8753-57DBF6EEF629}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C064456A-E08A-474B-8753-57DBF6EEF629}"/>
   </bookViews>
   <sheets>
     <sheet name="GLOVE_6B_50D" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="53">
   <si>
     <t xml:space="preserve"> activity</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>AUC</t>
+  </si>
+  <si>
+    <t>Number of Epochs</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Training Batch Size</t>
   </si>
 </sst>
 </file>
@@ -602,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2888C2-D671-4F49-A60B-7C2C5F84AC69}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,9 +622,12 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -625,8 +637,17 @@
       <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -636,8 +657,17 @@
       <c r="C2" s="3">
         <v>0.827653820148749</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>1E-4</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -647,8 +677,17 @@
       <c r="C3" s="3">
         <v>0.83589894387050001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3">
+        <v>1E-4</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -658,8 +697,17 @@
       <c r="C4" s="3">
         <v>0.811871949468848</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>1E-4</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -669,8 +717,17 @@
       <c r="C5" s="3">
         <v>0.87925458808311097</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>1E-4</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -680,8 +737,17 @@
       <c r="C6" s="3">
         <v>0.82785186945645395</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>1E-4</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -691,8 +757,17 @@
       <c r="C7" s="3">
         <v>0.78221217381013397</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>1E-4</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -702,8 +777,17 @@
       <c r="C8" s="3">
         <v>0.84276365108054196</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>5000</v>
+      </c>
+      <c r="E8">
+        <v>1E-4</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -713,8 +797,17 @@
       <c r="C9" s="3">
         <v>0.82560918298987096</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5000</v>
+      </c>
+      <c r="E9">
+        <v>1E-4</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -724,8 +817,17 @@
       <c r="C10" s="3">
         <v>0.86771402189684699</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -735,8 +837,17 @@
       <c r="C11" s="3">
         <v>0.84506047768158599</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>1E-4</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -746,8 +857,17 @@
       <c r="C12" s="3">
         <v>0.88589317068662699</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -757,8 +877,17 @@
       <c r="C13" s="3">
         <v>0.76071645919778696</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>5000</v>
+      </c>
+      <c r="E13">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -768,8 +897,17 @@
       <c r="C14" s="3">
         <v>0.932445725380044</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>5000</v>
+      </c>
+      <c r="E14">
+        <v>1E-4</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -779,8 +917,17 @@
       <c r="C15" s="3">
         <v>0.93264530845353</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>5000</v>
+      </c>
+      <c r="E15">
+        <v>1E-4</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -790,8 +937,17 @@
       <c r="C16" s="3">
         <v>0.80124396135265696</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>5000</v>
+      </c>
+      <c r="E16">
+        <v>1E-4</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -801,8 +957,17 @@
       <c r="C17" s="3">
         <v>0.87948030837075297</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>1E-4</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -812,8 +977,17 @@
       <c r="C18" s="3">
         <v>0.87948030837075297</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>5000</v>
+      </c>
+      <c r="E18">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -823,8 +997,17 @@
       <c r="C19" s="3">
         <v>0.912211433105376</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>1E-4</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -834,8 +1017,17 @@
       <c r="C20" s="3">
         <v>0.93237607809686196</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>1E-4</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -845,8 +1037,17 @@
       <c r="C21" s="3">
         <v>0.87004287925303803</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -856,8 +1057,17 @@
       <c r="C22" s="3">
         <v>0.81453792296147798</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>5000</v>
+      </c>
+      <c r="E22">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -867,8 +1077,17 @@
       <c r="C23" s="3">
         <v>0.84963496654586002</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -878,8 +1097,17 @@
       <c r="C24" s="3">
         <v>0.76717127827944998</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>5000</v>
+      </c>
+      <c r="E24">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -889,8 +1117,17 @@
       <c r="C25" s="3">
         <v>0.78794853963838596</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5000</v>
+      </c>
+      <c r="E25">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -900,8 +1137,17 @@
       <c r="C26" s="3">
         <v>0.93251968074259795</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -911,8 +1157,17 @@
       <c r="C27" s="3">
         <v>0.81013931743805501</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -922,8 +1177,17 @@
       <c r="C28" s="3">
         <v>0.80595529044077097</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -933,8 +1197,17 @@
       <c r="C29" s="3">
         <v>0.74215668207434304</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>5000</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -944,8 +1217,17 @@
       <c r="C30" s="3">
         <v>0.72486235267659804</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5000</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -955,8 +1237,17 @@
       <c r="C31" s="3">
         <v>0.80476725802222904</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -966,8 +1257,17 @@
       <c r="C32" s="5">
         <v>0.76199469296787403</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <v>1E-4</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -977,8 +1277,17 @@
       <c r="C33" s="3">
         <v>0.94626984328351804</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>1E-4</v>
+      </c>
+      <c r="F33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -988,8 +1297,17 @@
       <c r="C34" s="3">
         <v>0.76740733308062203</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34">
+        <v>1E-4</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -999,8 +1317,17 @@
       <c r="C35" s="5">
         <v>0.93234735756771503</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>5000</v>
+      </c>
+      <c r="E35">
+        <v>1E-4</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1010,8 +1337,17 @@
       <c r="C36" s="3">
         <v>0.93260871438295301</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36">
+        <v>1E-4</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1021,8 +1357,17 @@
       <c r="C37" s="5">
         <v>0.93247951932586703</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <v>1E-4</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1032,8 +1377,17 @@
       <c r="C38" s="3">
         <v>0.91825770942511697</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>1E-4</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1043,8 +1397,17 @@
       <c r="C39" s="4">
         <v>0.85462246357187899</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>5000</v>
+      </c>
+      <c r="E39">
+        <v>1E-4</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1054,8 +1417,17 @@
       <c r="C40" s="3">
         <v>0.90908443195275002</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>5000</v>
+      </c>
+      <c r="E40">
+        <v>1E-4</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1065,8 +1437,17 @@
       <c r="C41" s="4">
         <v>0.84238038004849003</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>5000</v>
+      </c>
+      <c r="E41">
+        <v>1E-4</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1076,8 +1457,17 @@
       <c r="C42" s="3">
         <v>0.80646413007494699</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>5000</v>
+      </c>
+      <c r="E42">
+        <v>1E-4</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1087,8 +1477,17 @@
       <c r="C43" s="5">
         <v>0.82564750163380196</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>5000</v>
+      </c>
+      <c r="E43">
+        <v>1E-4</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1098,8 +1497,17 @@
       <c r="C44" s="3">
         <v>0.79035369328052196</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>5000</v>
+      </c>
+      <c r="E44">
+        <v>1E-4</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1109,8 +1517,17 @@
       <c r="C45" s="5">
         <v>0.87906973865795301</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>5000</v>
+      </c>
+      <c r="E45">
+        <v>1E-4</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -1120,8 +1537,17 @@
       <c r="C46" s="3">
         <v>0.79934800518757598</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>5000</v>
+      </c>
+      <c r="E46">
+        <v>1E-4</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -1131,8 +1557,17 @@
       <c r="C47" s="3">
         <v>0.89746516383697095</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>5000</v>
+      </c>
+      <c r="E47">
+        <v>1E-4</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -1141,6 +1576,15 @@
       </c>
       <c r="C48" s="3">
         <v>0.83834223048087497</v>
+      </c>
+      <c r="D48">
+        <v>5000</v>
+      </c>
+      <c r="E48">
+        <v>1E-4</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1154,20 +1598,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541D66B4-0396-4EB2-B4BB-3E52838AA54C}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -1177,8 +1622,17 @@
       <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1188,8 +1642,17 @@
       <c r="C2" s="5">
         <v>0.87696899449434895</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>1E-4</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1199,8 +1662,17 @@
       <c r="C3" s="5">
         <v>0.88815912131780395</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3">
+        <v>1E-4</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1210,8 +1682,17 @@
       <c r="C4" s="5">
         <v>0.87958260318591697</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>1E-4</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1221,8 +1702,17 @@
       <c r="C5" s="5">
         <v>0.94879447723250698</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>1E-4</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1232,8 +1722,17 @@
       <c r="C6" s="5">
         <v>0.881511714001042</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>1E-4</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1243,8 +1742,17 @@
       <c r="C7" s="5">
         <v>0.83345496623865001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>1E-4</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1254,8 +1762,17 @@
       <c r="C8" s="5">
         <v>0.89842575090715904</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>5000</v>
+      </c>
+      <c r="E8">
+        <v>1E-4</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1265,8 +1782,17 @@
       <c r="C9" s="5">
         <v>0.86780704122546504</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5000</v>
+      </c>
+      <c r="E9">
+        <v>1E-4</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1276,8 +1802,17 @@
       <c r="C10" s="5">
         <v>0.90608099195356795</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1287,8 +1822,17 @@
       <c r="C11" s="5">
         <v>0.88926515248121396</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>1E-4</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1298,8 +1842,17 @@
       <c r="C12" s="5">
         <v>0.93930782737270102</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1309,8 +1862,17 @@
       <c r="C13" s="5">
         <v>0.85131950207468798</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>5000</v>
+      </c>
+      <c r="E13">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1320,8 +1882,17 @@
       <c r="C14" s="5">
         <v>0.96053512089906701</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>5000</v>
+      </c>
+      <c r="E14">
+        <v>1E-4</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1331,8 +1902,17 @@
       <c r="C15" s="5">
         <v>0.96080945112365002</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>5000</v>
+      </c>
+      <c r="E15">
+        <v>1E-4</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1342,8 +1922,17 @@
       <c r="C16" s="5">
         <v>0.86280434782608695</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>5000</v>
+      </c>
+      <c r="E16">
+        <v>1E-4</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1353,8 +1942,17 @@
       <c r="C17" s="5">
         <v>0.91939267378043799</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>1E-4</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1364,8 +1962,17 @@
       <c r="C18" s="5">
         <v>0.85676695757777799</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>5000</v>
+      </c>
+      <c r="E18">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1375,8 +1982,17 @@
       <c r="C19" s="5">
         <v>0.93864476937737895</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>1E-4</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1386,8 +2002,17 @@
       <c r="C20" s="5">
         <v>0.96051214447574895</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>1E-4</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1397,8 +2022,17 @@
       <c r="C21" s="5">
         <v>0.91077182655469002</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1408,8 +2042,17 @@
       <c r="C22" s="5">
         <v>0.84373523009648199</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>5000</v>
+      </c>
+      <c r="E22">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1419,8 +2062,17 @@
       <c r="C23" s="5">
         <v>0.905587886813493</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1430,8 +2082,17 @@
       <c r="C24" s="5">
         <v>0.83900496635222899</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>5000</v>
+      </c>
+      <c r="E24">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1441,8 +2102,17 @@
       <c r="C25" s="5">
         <v>0.88246175243393499</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5000</v>
+      </c>
+      <c r="E25">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1452,8 +2122,17 @@
       <c r="C26" s="5">
         <v>0.96053799295198194</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1463,8 +2142,17 @@
       <c r="C27" s="5">
         <v>0.86498924731182703</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1474,8 +2162,17 @@
       <c r="C28" s="5">
         <v>0.85371471237448604</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1485,8 +2182,17 @@
       <c r="C29" s="5">
         <v>0.79146662968317605</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>5000</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1496,8 +2202,17 @@
       <c r="C30" s="5">
         <v>0.74662314730006296</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5000</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1507,8 +2222,17 @@
       <c r="C31" s="5">
         <v>0.85577217186122001</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1518,8 +2242,17 @@
       <c r="C32" s="5">
         <v>0.821885043034982</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <v>1E-4</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1529,8 +2262,17 @@
       <c r="C33" s="5">
         <v>0.97193819298201101</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>1E-4</v>
+      </c>
+      <c r="F33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1540,8 +2282,17 @@
       <c r="C34" s="5">
         <v>0.84527393136664597</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34">
+        <v>1E-4</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1551,8 +2302,17 @@
       <c r="C35" s="5">
         <v>0.96049491215826099</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>5000</v>
+      </c>
+      <c r="E35">
+        <v>1E-4</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1562,8 +2322,17 @@
       <c r="C36" s="5">
         <v>0.96060117811610501</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36">
+        <v>1E-4</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1573,8 +2342,17 @@
       <c r="C37" s="5">
         <v>0.96088662882100995</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <v>1E-4</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1584,8 +2362,17 @@
       <c r="C38" s="5">
         <v>0.95727666148754798</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>1E-4</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1595,8 +2382,17 @@
       <c r="C39" s="5">
         <v>0.90305867932327</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>5000</v>
+      </c>
+      <c r="E39">
+        <v>1E-4</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1606,8 +2402,17 @@
       <c r="C40" s="5">
         <v>0.93165792848614004</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>5000</v>
+      </c>
+      <c r="E40">
+        <v>1E-4</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1617,8 +2422,17 @@
       <c r="C41" s="5">
         <v>0.89138363346250205</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>5000</v>
+      </c>
+      <c r="E41">
+        <v>1E-4</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1628,8 +2442,17 @@
       <c r="C42" s="5">
         <v>0.87388678139398501</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>5000</v>
+      </c>
+      <c r="E42">
+        <v>1E-4</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1639,8 +2462,17 @@
       <c r="C43" s="5">
         <v>0.90309955629370098</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>5000</v>
+      </c>
+      <c r="E43">
+        <v>1E-4</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1650,8 +2482,17 @@
       <c r="C44" s="5">
         <v>0.84673337502605694</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>5000</v>
+      </c>
+      <c r="E44">
+        <v>1E-4</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1661,8 +2502,17 @@
       <c r="C45" s="5">
         <v>0.91372711013744701</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>5000</v>
+      </c>
+      <c r="E45">
+        <v>1E-4</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -1672,8 +2522,17 @@
       <c r="C46" s="5">
         <v>0.86598628997607197</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>5000</v>
+      </c>
+      <c r="E46">
+        <v>1E-4</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -1683,8 +2542,17 @@
       <c r="C47" s="5">
         <v>0.93710899838735395</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>5000</v>
+      </c>
+      <c r="E47">
+        <v>1E-4</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -1693,6 +2561,15 @@
       </c>
       <c r="C48" s="5">
         <v>0.88326297963143896</v>
+      </c>
+      <c r="D48">
+        <v>5000</v>
+      </c>
+      <c r="E48">
+        <v>1E-4</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1709,10 +2586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90454682-D9A3-4462-9AB8-19A8B4E58653}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,9 +2597,12 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -1732,8 +2612,17 @@
       <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1743,8 +2632,17 @@
       <c r="C2" s="3">
         <v>0.91423162368395605</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>1E-4</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1754,8 +2652,17 @@
       <c r="C3" s="3">
         <v>0.91896426926367003</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3">
+        <v>1E-4</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1765,8 +2672,17 @@
       <c r="C4" s="3">
         <v>0.89370167414139601</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>1E-4</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1776,8 +2692,17 @@
       <c r="C5" s="3">
         <v>0.97091968271934304</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>1E-4</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1787,8 +2712,17 @@
       <c r="C6" s="3">
         <v>0.89652251544042105</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>1E-4</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1798,8 +2732,17 @@
       <c r="C7" s="3">
         <v>0.85533080862870403</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>1E-4</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1809,8 +2752,17 @@
       <c r="C8" s="3">
         <v>0.94157158165353605</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>5000</v>
+      </c>
+      <c r="E8">
+        <v>1E-4</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1820,8 +2772,17 @@
       <c r="C9" s="3">
         <v>0.89827368989411105</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5000</v>
+      </c>
+      <c r="E9">
+        <v>1E-4</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1831,8 +2792,17 @@
       <c r="C10" s="3">
         <v>0.94531855955678601</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1842,8 +2812,17 @@
       <c r="C11" s="3">
         <v>0.91790054361430296</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>1E-4</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1853,8 +2832,17 @@
       <c r="C12" s="3">
         <v>0.96046268059021001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1864,8 +2852,17 @@
       <c r="C13" s="3">
         <v>0.920716459197787</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>5000</v>
+      </c>
+      <c r="E13">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1875,8 +2872,17 @@
       <c r="C14" s="3">
         <v>0.96741512365623805</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>5000</v>
+      </c>
+      <c r="E14">
+        <v>1E-4</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1886,8 +2892,17 @@
       <c r="C15" s="3">
         <v>0.96762967282373102</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>5000</v>
+      </c>
+      <c r="E15">
+        <v>1E-4</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1897,8 +2912,17 @@
       <c r="C16" s="3">
         <v>0.90607004830917803</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>5000</v>
+      </c>
+      <c r="E16">
+        <v>1E-4</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1908,8 +2932,17 @@
       <c r="C17" s="3">
         <v>0.95002052049635399</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>1E-4</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1919,8 +2952,17 @@
       <c r="C18" s="3">
         <v>0.89587525350541897</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>5000</v>
+      </c>
+      <c r="E18">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1930,8 +2972,17 @@
       <c r="C19" s="3">
         <v>0.96216462429104499</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>1E-4</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1941,8 +2992,17 @@
       <c r="C20" s="3">
         <v>0.96734906643920004</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>1E-4</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1952,8 +3012,17 @@
       <c r="C21" s="3">
         <v>0.93949331438865302</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1963,8 +3032,17 @@
       <c r="C22" s="5">
         <v>0.86758753170875702</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>5000</v>
+      </c>
+      <c r="E22">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1974,8 +3052,17 @@
       <c r="C23" s="5">
         <v>0.93180451979369905</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1985,8 +3072,17 @@
       <c r="C24" s="5">
         <v>0.86981062371170803</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>5000</v>
+      </c>
+      <c r="E24">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1996,8 +3092,17 @@
       <c r="C25" s="5">
         <v>0.91937644877144098</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5000</v>
+      </c>
+      <c r="E25">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2007,8 +3112,17 @@
       <c r="C26" s="5">
         <v>0.96742948392081096</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2018,8 +3132,17 @@
       <c r="C27" s="5">
         <v>0.90148480598410397</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -2029,8 +3152,17 @@
       <c r="C28" s="5">
         <v>0.881824450310698</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2040,8 +3172,17 @@
       <c r="C29" s="3">
         <v>0.78395055864701202</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>5000</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2051,8 +3192,17 @@
       <c r="C30" s="3">
         <v>0.76589134787386903</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5000</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2062,8 +3212,17 @@
       <c r="C31" s="3">
         <v>0.85537691965456097</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2073,8 +3232,17 @@
       <c r="C32" s="3">
         <v>0.87387487224951599</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <v>1E-4</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -2084,8 +3252,17 @@
       <c r="C33" s="3">
         <v>0.98095383080032805</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>1E-4</v>
+      </c>
+      <c r="F33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -2095,8 +3272,17 @@
       <c r="C34" s="3">
         <v>0.88653644613909499</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34">
+        <v>1E-4</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2106,8 +3292,17 @@
       <c r="C35" s="3">
         <v>0.96739214723292</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>5000</v>
+      </c>
+      <c r="E35">
+        <v>1E-4</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2117,8 +3312,17 @@
       <c r="C36" s="4">
         <v>0.96742230378852501</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36">
+        <v>1E-4</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -2128,8 +3332,17 @@
       <c r="C37" s="3">
         <v>0.96752391079401501</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <v>1E-4</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2139,8 +3352,17 @@
       <c r="C38" s="3">
         <v>0.97916063167689305</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>1E-4</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -2150,8 +3372,17 @@
       <c r="C39" s="3">
         <v>0.93598532898143805</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>5000</v>
+      </c>
+      <c r="E39">
+        <v>1E-4</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -2161,8 +3392,17 @@
       <c r="C40" s="3">
         <v>0.96228496459685597</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>5000</v>
+      </c>
+      <c r="E40">
+        <v>1E-4</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2172,8 +3412,17 @@
       <c r="C41" s="3">
         <v>0.93976003481360204</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>5000</v>
+      </c>
+      <c r="E41">
+        <v>1E-4</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2183,8 +3432,17 @@
       <c r="C42" s="3">
         <v>0.91807633654070497</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>5000</v>
+      </c>
+      <c r="E42">
+        <v>1E-4</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2194,8 +3452,17 @@
       <c r="C43" s="3">
         <v>0.93771650951044805</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>5000</v>
+      </c>
+      <c r="E43">
+        <v>1E-4</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2205,8 +3472,17 @@
       <c r="C44" s="3">
         <v>0.869418386491557</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>5000</v>
+      </c>
+      <c r="E44">
+        <v>1E-4</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2216,8 +3492,17 @@
       <c r="C45" s="3">
         <v>0.93739363446769197</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>5000</v>
+      </c>
+      <c r="E45">
+        <v>1E-4</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2227,8 +3512,17 @@
       <c r="C46" s="3">
         <v>0.90157795358774495</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>5000</v>
+      </c>
+      <c r="E46">
+        <v>1E-4</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2238,8 +3532,17 @@
       <c r="C47" s="3">
         <v>0.95396395111047705</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>5000</v>
+      </c>
+      <c r="E47">
+        <v>1E-4</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -2248,6 +3551,15 @@
       </c>
       <c r="C48" s="3">
         <v>0.92469110607476401</v>
+      </c>
+      <c r="D48">
+        <v>5000</v>
+      </c>
+      <c r="E48">
+        <v>1E-4</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2261,10 +3573,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6618C6B-8A06-4543-A082-B1EF35FE3E93}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,9 +3584,12 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -2284,8 +3599,17 @@
       <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -2295,8 +3619,17 @@
       <c r="C2" s="3">
         <v>0.94253066743938896</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>1E-4</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2306,8 +3639,17 @@
       <c r="C3" s="3">
         <v>0.94266823495865404</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3">
+        <v>1E-4</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2317,8 +3659,17 @@
       <c r="C4" s="3">
         <v>0.91637089508647895</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>1E-4</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2328,8 +3679,17 @@
       <c r="C5" s="3">
         <v>0.98777409473504496</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>1E-4</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2339,8 +3699,17 @@
       <c r="C6" s="3">
         <v>0.92331587430719897</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>1E-4</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2350,8 +3719,17 @@
       <c r="C7" s="3">
         <v>0.87604127629078798</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>1E-4</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2361,8 +3739,17 @@
       <c r="C8" s="3">
         <v>0.96004589835216603</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>5000</v>
+      </c>
+      <c r="E8">
+        <v>1E-4</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2372,8 +3759,17 @@
       <c r="C9" s="3">
         <v>0.93923918368979398</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5000</v>
+      </c>
+      <c r="E9">
+        <v>1E-4</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2383,8 +3779,17 @@
       <c r="C10" s="3">
         <v>0.96717847249703204</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2394,8 +3799,17 @@
       <c r="C11" s="3">
         <v>0.93952940287440201</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>1E-4</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2405,8 +3819,17 @@
       <c r="C12" s="3">
         <v>0.98266231299222695</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2416,8 +3839,17 @@
       <c r="C13" s="3">
         <v>0.96089349930843704</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>5000</v>
+      </c>
+      <c r="E13">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2427,8 +3859,17 @@
       <c r="C14" s="3">
         <v>0.97506627262100598</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>5000</v>
+      </c>
+      <c r="E14">
+        <v>1E-4</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2438,8 +3879,17 @@
       <c r="C15" s="4">
         <v>0.97493154052400699</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>5000</v>
+      </c>
+      <c r="E15">
+        <v>1E-4</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2449,8 +3899,17 @@
       <c r="C16" s="3">
         <v>0.95278260869565201</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>5000</v>
+      </c>
+      <c r="E16">
+        <v>1E-4</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2460,8 +3919,17 @@
       <c r="C17" s="3">
         <v>0.96911262935959896</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>1E-4</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2471,8 +3939,17 @@
       <c r="C18" s="3">
         <v>0.94160544833251902</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>5000</v>
+      </c>
+      <c r="E18">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2482,8 +3959,17 @@
       <c r="C19" s="3">
         <v>0.98494141551533698</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>1E-4</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2493,8 +3979,17 @@
       <c r="C20" s="3">
         <v>0.97477332322370702</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>1E-4</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2504,8 +3999,17 @@
       <c r="C21" s="3">
         <v>0.968360693172303</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2515,8 +4019,17 @@
       <c r="C22" s="3">
         <v>0.88779340716828303</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>5000</v>
+      </c>
+      <c r="E22">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2526,8 +4039,17 @@
       <c r="C23" s="3">
         <v>0.95931924310008299</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2537,8 +4059,17 @@
       <c r="C24" s="4">
         <v>0.92405847113596296</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>5000</v>
+      </c>
+      <c r="E24">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2548,8 +4079,17 @@
       <c r="C25" s="3">
         <v>0.94257765414928096</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5000</v>
+      </c>
+      <c r="E25">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2559,8 +4099,17 @@
       <c r="C26" s="3">
         <v>0.97495139050441804</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2570,8 +4119,17 @@
       <c r="C27" s="3">
         <v>0.923547452080411</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -2581,8 +4139,17 @@
       <c r="C28" s="3">
         <v>0.92707870073808696</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2592,8 +4159,17 @@
       <c r="C29" s="3">
         <v>0.80029422139304895</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>5000</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2603,8 +4179,17 @@
       <c r="C30" s="3">
         <v>0.77964153199970598</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5000</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2614,8 +4199,17 @@
       <c r="C31" s="3">
         <v>0.87536545932676002</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2625,8 +4219,17 @@
       <c r="C32" s="3">
         <v>0.90466427788654502</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <v>1E-4</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -2636,8 +4239,17 @@
       <c r="C33" s="3">
         <v>0.99395926893833597</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>1E-4</v>
+      </c>
+      <c r="F33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -2647,8 +4259,17 @@
       <c r="C34" s="3">
         <v>0.91534736623036805</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34">
+        <v>1E-4</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2658,8 +4279,17 @@
       <c r="C35" s="3">
         <v>0.97490974573715505</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>5000</v>
+      </c>
+      <c r="E35">
+        <v>1E-4</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2669,8 +4299,17 @@
       <c r="C36" s="3">
         <v>0.97487528110217903</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36">
+        <v>1E-4</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -2680,8 +4319,17 @@
       <c r="C37" s="3">
         <v>0.97517307813241305</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <v>1E-4</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2691,8 +4339,17 @@
       <c r="C38" s="3">
         <v>0.98774348440558601</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>1E-4</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -2702,8 +4359,17 @@
       <c r="C39" s="3">
         <v>0.96770047937363102</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>5000</v>
+      </c>
+      <c r="E39">
+        <v>1E-4</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -2713,8 +4379,17 @@
       <c r="C40" s="3">
         <v>0.98189304860131699</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>5000</v>
+      </c>
+      <c r="E40">
+        <v>1E-4</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2724,8 +4399,17 @@
       <c r="C41" s="3">
         <v>0.96924021385498405</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>5000</v>
+      </c>
+      <c r="E41">
+        <v>1E-4</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2735,8 +4419,17 @@
       <c r="C42" s="3">
         <v>0.95157736496203804</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>5000</v>
+      </c>
+      <c r="E42">
+        <v>1E-4</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2746,8 +4439,17 @@
       <c r="C43" s="3">
         <v>0.96644440404298404</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>5000</v>
+      </c>
+      <c r="E43">
+        <v>1E-4</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2757,8 +4459,17 @@
       <c r="C44" s="3">
         <v>0.90306580501702405</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>5000</v>
+      </c>
+      <c r="E44">
+        <v>1E-4</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2768,8 +4479,17 @@
       <c r="C45" s="3">
         <v>0.957871513531242</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>5000</v>
+      </c>
+      <c r="E45">
+        <v>1E-4</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2779,8 +4499,17 @@
       <c r="C46" s="3">
         <v>0.93247478151866603</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>5000</v>
+      </c>
+      <c r="E46">
+        <v>1E-4</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2790,8 +4519,17 @@
       <c r="C47" s="3">
         <v>0.98007972433710699</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>5000</v>
+      </c>
+      <c r="E47">
+        <v>1E-4</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -2800,6 +4538,15 @@
       </c>
       <c r="C48" s="3">
         <v>0.94644883871637597</v>
+      </c>
+      <c r="D48">
+        <v>5000</v>
+      </c>
+      <c r="E48">
+        <v>1E-4</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2807,25 +4554,11 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x0101007D6227B7D589F74C87E894009163A6E9" ma:contentTypeVersion="7" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="cce2196116002440e3ec2c98653be481">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="540722d3-99d9-4277-bac4-fa26ca6f3e31" xmlns:ns4="eb6c88fb-620c-4a1e-a860-b962f6518fbf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d51ebdfc1605152fc236cccd0da138f2" ns3:_="" ns4:_="">
     <xsd:import namespace="540722d3-99d9-4277-bac4-fa26ca6f3e31"/>
@@ -3010,32 +4743,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B44AB92-5CC8-44CE-8040-69092FA17F11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="540722d3-99d9-4277-bac4-fa26ca6f3e31"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="eb6c88fb-620c-4a1e-a860-b962f6518fbf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5A5093-2B01-4C2B-A48A-0787FE3E98DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7055609F-A39A-4A86-8DF8-F6AEAAEE44AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3052,4 +4775,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5A5093-2B01-4C2B-A48A-0787FE3E98DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B44AB92-5CC8-44CE-8040-69092FA17F11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="540722d3-99d9-4277-bac4-fa26ca6f3e31"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="eb6c88fb-620c-4a1e-a860-b962f6518fbf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>